<commit_message>
AFTER BOXPLOT AND DELETE FORUM
</commit_message>
<xml_diff>
--- a/Users_to_try.xlsx
+++ b/Users_to_try.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VS\Carpetas\Entrega_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1BB083-BC98-43B8-898A-412860208E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9085059-9A37-4761-90E7-F45151CB1ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Usuario</t>
   </si>
@@ -378,7 +389,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,6 +449,9 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>